<commit_message>
Reduced conditional checks in difference calculation
Converted some data from lists to frozensets in difference calculations. Also stored rows to iterate over as a list, instead of looping over list of all possible rows and checking each to see if it is in df.
</commit_message>
<xml_diff>
--- a/output/grahade01.xlsx
+++ b/output/grahade01.xlsx
@@ -25,7 +25,7 @@
     <t>Age</t>
   </si>
   <si>
-    <t>Tm</t>
+    <t>Team</t>
   </si>
   <si>
     <t>Lg</t>
@@ -2448,7 +2448,7 @@
         <v>10.6</v>
       </c>
       <c r="T6">
-        <v>21.5</v>
+        <v>21.4</v>
       </c>
       <c r="V6">
         <v>2</v>
@@ -2460,7 +2460,7 @@
         <v>2.9</v>
       </c>
       <c r="Y6">
-        <v>0.091</v>
+        <v>0.092</v>
       </c>
       <c r="AA6">
         <v>1.2</v>

</xml_diff>

<commit_message>
fixed previous change that caused rsvsps to scrape each page multiple times leading to 429 errors
</commit_message>
<xml_diff>
--- a/output/grahade01.xlsx
+++ b/output/grahade01.xlsx
@@ -1299,13 +1299,13 @@
         <v>50</v>
       </c>
       <c r="G11">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H11">
         <v>6</v>
       </c>
       <c r="I11">
-        <v>17.9</v>
+        <v>18</v>
       </c>
       <c r="J11">
         <v>2.2</v>
@@ -1314,28 +1314,28 @@
         <v>5.8</v>
       </c>
       <c r="L11">
-        <v>0.382</v>
+        <v>0.375</v>
       </c>
       <c r="M11">
-        <v>1.7</v>
+        <v>1.6</v>
       </c>
       <c r="N11">
         <v>4.6</v>
       </c>
       <c r="O11">
-        <v>0.362</v>
+        <v>0.354</v>
       </c>
       <c r="P11">
         <v>0.6</v>
       </c>
       <c r="Q11">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="R11">
-        <v>0.458</v>
+        <v>0.448</v>
       </c>
       <c r="S11">
-        <v>0.524</v>
+        <v>0.514</v>
       </c>
       <c r="T11">
         <v>1.3</v>
@@ -1344,7 +1344,7 @@
         <v>1.7</v>
       </c>
       <c r="V11">
-        <v>0.759</v>
+        <v>0.763</v>
       </c>
       <c r="W11">
         <v>0.3</v>
@@ -1353,10 +1353,10 @@
         <v>1.4</v>
       </c>
       <c r="Y11">
-        <v>1.6</v>
+        <v>1.7</v>
       </c>
       <c r="Z11">
-        <v>2.6</v>
+        <v>2.7</v>
       </c>
       <c r="AA11">
         <v>0.6</v>
@@ -1371,7 +1371,7 @@
         <v>1.1</v>
       </c>
       <c r="AE11">
-        <v>7.4</v>
+        <v>7.3</v>
       </c>
       <c r="AF11" t="s">
         <v>51</v>
@@ -1495,70 +1495,70 @@
         <v>50</v>
       </c>
       <c r="G13">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H13">
         <v>6</v>
       </c>
       <c r="I13">
-        <v>27.9</v>
+        <v>27.1</v>
       </c>
       <c r="J13">
-        <v>4.6</v>
+        <v>4.1</v>
       </c>
       <c r="K13">
-        <v>11.4</v>
+        <v>10.8</v>
       </c>
       <c r="L13">
-        <v>0.403</v>
+        <v>0.384</v>
       </c>
       <c r="M13">
-        <v>3.2</v>
+        <v>2.9</v>
       </c>
       <c r="N13">
-        <v>8.4</v>
+        <v>7.9</v>
       </c>
       <c r="O13">
-        <v>0.385</v>
+        <v>0.365</v>
       </c>
       <c r="P13">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="Q13">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="R13">
-        <v>0.452</v>
+        <v>0.435</v>
       </c>
       <c r="S13">
-        <v>0.544</v>
+        <v>0.517</v>
       </c>
       <c r="T13">
-        <v>3.1</v>
+        <v>2.9</v>
       </c>
       <c r="U13">
-        <v>4.1</v>
+        <v>3.7</v>
       </c>
       <c r="V13">
-        <v>0.772</v>
+        <v>0.78</v>
       </c>
       <c r="W13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X13">
         <v>2.2</v>
       </c>
       <c r="Y13">
-        <v>2.7</v>
+        <v>2.6</v>
       </c>
       <c r="Z13">
-        <v>4.4</v>
+        <v>4.3</v>
       </c>
       <c r="AA13">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="AB13">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="AC13">
         <v>1.4</v>
@@ -1567,7 +1567,7 @@
         <v>1.6</v>
       </c>
       <c r="AE13">
-        <v>15.5</v>
+        <v>14</v>
       </c>
       <c r="AF13" t="s">
         <v>51</v>
@@ -1944,70 +1944,70 @@
         <v>49</v>
       </c>
       <c r="G20">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H20">
         <v>6</v>
       </c>
       <c r="I20">
-        <v>27.9</v>
+        <v>27.1</v>
       </c>
       <c r="J20">
-        <v>4.6</v>
+        <v>4.1</v>
       </c>
       <c r="K20">
-        <v>11.4</v>
+        <v>10.8</v>
       </c>
       <c r="L20">
-        <v>0.403</v>
+        <v>0.384</v>
       </c>
       <c r="M20">
-        <v>3.2</v>
+        <v>2.9</v>
       </c>
       <c r="N20">
-        <v>8.4</v>
+        <v>7.9</v>
       </c>
       <c r="O20">
-        <v>0.385</v>
+        <v>0.365</v>
       </c>
       <c r="P20">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="Q20">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="R20">
-        <v>0.452</v>
+        <v>0.435</v>
       </c>
       <c r="S20">
-        <v>0.544</v>
+        <v>0.517</v>
       </c>
       <c r="T20">
-        <v>3.1</v>
+        <v>2.9</v>
       </c>
       <c r="U20">
-        <v>4.1</v>
+        <v>3.7</v>
       </c>
       <c r="V20">
-        <v>0.772</v>
+        <v>0.78</v>
       </c>
       <c r="W20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X20">
         <v>2.2</v>
       </c>
       <c r="Y20">
-        <v>2.7</v>
+        <v>2.6</v>
       </c>
       <c r="Z20">
-        <v>4.4</v>
+        <v>4.3</v>
       </c>
       <c r="AA20">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="AB20">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="AC20">
         <v>1.4</v>
@@ -2016,7 +2016,7 @@
         <v>1.6</v>
       </c>
       <c r="AE20">
-        <v>15.5</v>
+        <v>14</v>
       </c>
       <c r="AF20" t="s">
         <v>51</v>
@@ -2038,13 +2038,13 @@
         <v>49</v>
       </c>
       <c r="G22">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="H22">
         <v>169</v>
       </c>
       <c r="I22">
-        <v>25.8</v>
+        <v>25.7</v>
       </c>
       <c r="J22">
         <v>3.7</v>
@@ -2053,7 +2053,7 @@
         <v>9.9</v>
       </c>
       <c r="L22">
-        <v>0.373</v>
+        <v>0.372</v>
       </c>
       <c r="M22">
         <v>2.4</v>
@@ -2062,28 +2062,28 @@
         <v>6.7</v>
       </c>
       <c r="O22">
-        <v>0.358</v>
+        <v>0.356</v>
       </c>
       <c r="P22">
         <v>1.3</v>
       </c>
       <c r="Q22">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="R22">
-        <v>0.405</v>
+        <v>0.404</v>
       </c>
       <c r="S22">
-        <v>0.493</v>
+        <v>0.492</v>
       </c>
       <c r="T22">
         <v>1.8</v>
       </c>
       <c r="U22">
-        <v>2.3</v>
+        <v>2.2</v>
       </c>
       <c r="V22">
-        <v>0.8149999999999999</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="W22">
         <v>0.4</v>
@@ -2110,7 +2110,7 @@
         <v>1.3</v>
       </c>
       <c r="AE22">
-        <v>11.7</v>
+        <v>11.6</v>
       </c>
       <c r="AF22" t="s">
         <v>51</v>
@@ -2216,7 +2216,7 @@
         <v>-6.9</v>
       </c>
       <c r="L24">
-        <v>-0.03999999999999998</v>
+        <v>-0.03899999999999998</v>
       </c>
       <c r="M24">
         <v>-1.6</v>
@@ -2225,28 +2225,28 @@
         <v>-4.4</v>
       </c>
       <c r="O24">
-        <v>-0.001000000000000001</v>
+        <v>0.001000000000000001</v>
       </c>
       <c r="P24">
         <v>-1.1</v>
       </c>
       <c r="Q24">
-        <v>-2.6</v>
+        <v>-2.5</v>
       </c>
       <c r="R24">
-        <v>-0.155</v>
+        <v>-0.154</v>
       </c>
       <c r="S24">
-        <v>-0.02100000000000002</v>
+        <v>-0.02000000000000002</v>
       </c>
       <c r="T24">
         <v>-0.6000000000000001</v>
       </c>
       <c r="U24">
-        <v>-0.9999999999999998</v>
+        <v>-0.9000000000000001</v>
       </c>
       <c r="V24">
-        <v>0.06000000000000005</v>
+        <v>0.05900000000000005</v>
       </c>
       <c r="W24">
         <v>-0.1</v>
@@ -2273,7 +2273,7 @@
         <v>-0.8</v>
       </c>
       <c r="AE24">
-        <v>-7.699999999999999</v>
+        <v>-7.6</v>
       </c>
     </row>
   </sheetData>
@@ -2959,31 +2959,31 @@
         <v>50</v>
       </c>
       <c r="G11">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H11">
         <v>6</v>
       </c>
       <c r="I11">
-        <v>1202</v>
+        <v>1245</v>
       </c>
       <c r="J11">
-        <v>4.5</v>
+        <v>4.4</v>
       </c>
       <c r="K11">
         <v>11.7</v>
       </c>
       <c r="L11">
-        <v>0.382</v>
+        <v>0.375</v>
       </c>
       <c r="M11">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="N11">
-        <v>9.199999999999999</v>
+        <v>9.1</v>
       </c>
       <c r="O11">
-        <v>0.362</v>
+        <v>0.354</v>
       </c>
       <c r="P11">
         <v>1.1</v>
@@ -2992,19 +2992,19 @@
         <v>2.5</v>
       </c>
       <c r="R11">
-        <v>0.458</v>
+        <v>0.448</v>
       </c>
       <c r="S11">
         <v>2.6</v>
       </c>
       <c r="T11">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="U11">
-        <v>0.759</v>
+        <v>0.763</v>
       </c>
       <c r="V11">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="W11">
         <v>2.7</v>
@@ -3028,7 +3028,7 @@
         <v>2.1</v>
       </c>
       <c r="AD11">
-        <v>14.9</v>
+        <v>14.6</v>
       </c>
       <c r="AE11" t="s">
         <v>51</v>
@@ -3149,49 +3149,49 @@
         <v>50</v>
       </c>
       <c r="G13">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H13">
         <v>6</v>
       </c>
       <c r="I13">
-        <v>391</v>
+        <v>434</v>
       </c>
       <c r="J13">
-        <v>5.9</v>
+        <v>5.5</v>
       </c>
       <c r="K13">
-        <v>14.6</v>
+        <v>14.3</v>
       </c>
       <c r="L13">
-        <v>0.403</v>
+        <v>0.384</v>
       </c>
       <c r="M13">
-        <v>4.1</v>
+        <v>3.8</v>
       </c>
       <c r="N13">
-        <v>10.8</v>
+        <v>10.5</v>
       </c>
       <c r="O13">
-        <v>0.385</v>
+        <v>0.365</v>
       </c>
       <c r="P13">
         <v>1.7</v>
       </c>
       <c r="Q13">
-        <v>3.9</v>
+        <v>3.8</v>
       </c>
       <c r="R13">
-        <v>0.452</v>
+        <v>0.435</v>
       </c>
       <c r="S13">
-        <v>4.1</v>
+        <v>3.8</v>
       </c>
       <c r="T13">
-        <v>5.2</v>
+        <v>4.9</v>
       </c>
       <c r="U13">
-        <v>0.772</v>
+        <v>0.78</v>
       </c>
       <c r="V13">
         <v>0.6</v>
@@ -3206,19 +3206,19 @@
         <v>5.6</v>
       </c>
       <c r="Z13">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="AA13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB13">
-        <v>1.7</v>
+        <v>1.8</v>
       </c>
       <c r="AC13">
-        <v>2.1</v>
+        <v>2.2</v>
       </c>
       <c r="AD13">
-        <v>20</v>
+        <v>18.6</v>
       </c>
       <c r="AE13" t="s">
         <v>51</v>
@@ -3583,49 +3583,49 @@
         <v>49</v>
       </c>
       <c r="G20">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H20">
         <v>6</v>
       </c>
       <c r="I20">
-        <v>391</v>
+        <v>434</v>
       </c>
       <c r="J20">
-        <v>5.9</v>
+        <v>5.5</v>
       </c>
       <c r="K20">
-        <v>14.6</v>
+        <v>14.3</v>
       </c>
       <c r="L20">
-        <v>0.403</v>
+        <v>0.384</v>
       </c>
       <c r="M20">
-        <v>4.1</v>
+        <v>3.8</v>
       </c>
       <c r="N20">
-        <v>10.8</v>
+        <v>10.5</v>
       </c>
       <c r="O20">
-        <v>0.385</v>
+        <v>0.365</v>
       </c>
       <c r="P20">
         <v>1.7</v>
       </c>
       <c r="Q20">
-        <v>3.9</v>
+        <v>3.8</v>
       </c>
       <c r="R20">
-        <v>0.452</v>
+        <v>0.435</v>
       </c>
       <c r="S20">
-        <v>4.1</v>
+        <v>3.8</v>
       </c>
       <c r="T20">
-        <v>5.2</v>
+        <v>4.9</v>
       </c>
       <c r="U20">
-        <v>0.772</v>
+        <v>0.78</v>
       </c>
       <c r="V20">
         <v>0.6</v>
@@ -3640,19 +3640,19 @@
         <v>5.6</v>
       </c>
       <c r="Z20">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="AA20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB20">
-        <v>1.7</v>
+        <v>1.8</v>
       </c>
       <c r="AC20">
-        <v>2.1</v>
+        <v>2.2</v>
       </c>
       <c r="AD20">
-        <v>20</v>
+        <v>18.6</v>
       </c>
       <c r="AE20" t="s">
         <v>51</v>
@@ -3674,13 +3674,13 @@
         <v>49</v>
       </c>
       <c r="G22">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="H22">
         <v>169</v>
       </c>
       <c r="I22">
-        <v>7910</v>
+        <v>7953</v>
       </c>
       <c r="J22">
         <v>5.2</v>
@@ -3689,7 +3689,7 @@
         <v>13.9</v>
       </c>
       <c r="L22">
-        <v>0.373</v>
+        <v>0.372</v>
       </c>
       <c r="M22">
         <v>3.3</v>
@@ -3698,25 +3698,25 @@
         <v>9.300000000000001</v>
       </c>
       <c r="O22">
-        <v>0.358</v>
+        <v>0.356</v>
       </c>
       <c r="P22">
         <v>1.8</v>
       </c>
       <c r="Q22">
-        <v>4.6</v>
+        <v>4.5</v>
       </c>
       <c r="R22">
-        <v>0.405</v>
+        <v>0.404</v>
       </c>
       <c r="S22">
         <v>2.6</v>
       </c>
       <c r="T22">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="U22">
-        <v>0.8149999999999999</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="V22">
         <v>0.6</v>
@@ -3740,10 +3740,10 @@
         <v>2</v>
       </c>
       <c r="AC22">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="AD22">
-        <v>16.3</v>
+        <v>16.2</v>
       </c>
       <c r="AE22" t="s">
         <v>51</v>
@@ -3846,7 +3846,7 @@
         <v>-3.1</v>
       </c>
       <c r="L24">
-        <v>-0.03999999999999998</v>
+        <v>-0.03899999999999998</v>
       </c>
       <c r="M24">
         <v>-0.2999999999999998</v>
@@ -3855,25 +3855,25 @@
         <v>-0.9000000000000004</v>
       </c>
       <c r="O24">
-        <v>-0.001000000000000001</v>
+        <v>0.001000000000000001</v>
       </c>
       <c r="P24">
         <v>-1.2</v>
       </c>
       <c r="Q24">
-        <v>-2.2</v>
+        <v>-2.1</v>
       </c>
       <c r="R24">
-        <v>-0.155</v>
+        <v>-0.154</v>
       </c>
       <c r="S24">
         <v>1.6</v>
       </c>
       <c r="T24">
-        <v>1.6</v>
+        <v>1.7</v>
       </c>
       <c r="U24">
-        <v>0.06000000000000005</v>
+        <v>0.05900000000000005</v>
       </c>
       <c r="V24">
         <v>0.6</v>
@@ -3897,10 +3897,10 @@
         <v>0.3999999999999999</v>
       </c>
       <c r="AC24">
-        <v>0</v>
+        <v>-0.09999999999999987</v>
       </c>
       <c r="AD24">
-        <v>-1.9</v>
+        <v>-1.799999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -4629,40 +4629,40 @@
         <v>50</v>
       </c>
       <c r="G11">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H11">
         <v>6</v>
       </c>
       <c r="I11">
-        <v>1202</v>
+        <v>1245</v>
       </c>
       <c r="J11">
-        <v>6</v>
+        <v>5.8</v>
       </c>
       <c r="K11">
-        <v>15.6</v>
+        <v>15.5</v>
       </c>
       <c r="L11">
-        <v>0.382</v>
+        <v>0.375</v>
       </c>
       <c r="M11">
-        <v>4.4</v>
+        <v>4.3</v>
       </c>
       <c r="N11">
-        <v>12.3</v>
+        <v>12.2</v>
       </c>
       <c r="O11">
-        <v>0.362</v>
+        <v>0.354</v>
       </c>
       <c r="P11">
         <v>1.5</v>
       </c>
       <c r="Q11">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="R11">
-        <v>0.458</v>
+        <v>0.448</v>
       </c>
       <c r="S11">
         <v>3.5</v>
@@ -4671,13 +4671,13 @@
         <v>4.6</v>
       </c>
       <c r="U11">
-        <v>0.759</v>
+        <v>0.763</v>
       </c>
       <c r="V11">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="W11">
-        <v>3.6</v>
+        <v>3.7</v>
       </c>
       <c r="X11">
         <v>4.4</v>
@@ -4692,16 +4692,16 @@
         <v>0.6</v>
       </c>
       <c r="AB11">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="AC11">
-        <v>2.8</v>
+        <v>2.9</v>
       </c>
       <c r="AD11">
-        <v>19.9</v>
+        <v>19.4</v>
       </c>
       <c r="AF11">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AG11">
         <v>117</v>
@@ -4831,49 +4831,49 @@
         <v>50</v>
       </c>
       <c r="G13">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H13">
         <v>6</v>
       </c>
       <c r="I13">
-        <v>391</v>
+        <v>434</v>
       </c>
       <c r="J13">
-        <v>7.8</v>
+        <v>7.2</v>
       </c>
       <c r="K13">
-        <v>19.3</v>
+        <v>18.8</v>
       </c>
       <c r="L13">
-        <v>0.403</v>
+        <v>0.384</v>
       </c>
       <c r="M13">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="N13">
-        <v>14.2</v>
+        <v>13.8</v>
       </c>
       <c r="O13">
-        <v>0.385</v>
+        <v>0.365</v>
       </c>
       <c r="P13">
-        <v>2.3</v>
+        <v>2.2</v>
       </c>
       <c r="Q13">
-        <v>5.1</v>
+        <v>5</v>
       </c>
       <c r="R13">
-        <v>0.452</v>
+        <v>0.435</v>
       </c>
       <c r="S13">
-        <v>5.3</v>
+        <v>5</v>
       </c>
       <c r="T13">
-        <v>6.9</v>
+        <v>6.4</v>
       </c>
       <c r="U13">
-        <v>0.772</v>
+        <v>0.78</v>
       </c>
       <c r="V13">
         <v>0.8</v>
@@ -4888,22 +4888,22 @@
         <v>7.4</v>
       </c>
       <c r="Z13">
-        <v>1.1</v>
+        <v>1.3</v>
       </c>
       <c r="AA13">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="AB13">
-        <v>2.3</v>
+        <v>2.4</v>
       </c>
       <c r="AC13">
         <v>2.8</v>
       </c>
       <c r="AD13">
-        <v>26.3</v>
+        <v>24.4</v>
       </c>
       <c r="AF13">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AG13">
         <v>122</v>
@@ -5103,7 +5103,7 @@
         <v>19.5</v>
       </c>
       <c r="AF17">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AG17">
         <v>116</v>
@@ -5275,7 +5275,7 @@
         <v>1.100000000000001</v>
       </c>
       <c r="AF19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG19">
         <v>4</v>
@@ -5295,49 +5295,49 @@
         <v>49</v>
       </c>
       <c r="G20">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H20">
         <v>6</v>
       </c>
       <c r="I20">
-        <v>391</v>
+        <v>434</v>
       </c>
       <c r="J20">
-        <v>7.8</v>
+        <v>7.2</v>
       </c>
       <c r="K20">
-        <v>19.3</v>
+        <v>18.8</v>
       </c>
       <c r="L20">
-        <v>0.403</v>
+        <v>0.384</v>
       </c>
       <c r="M20">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="N20">
-        <v>14.2</v>
+        <v>13.8</v>
       </c>
       <c r="O20">
-        <v>0.385</v>
+        <v>0.365</v>
       </c>
       <c r="P20">
-        <v>2.3</v>
+        <v>2.2</v>
       </c>
       <c r="Q20">
-        <v>5.1</v>
+        <v>5</v>
       </c>
       <c r="R20">
-        <v>0.452</v>
+        <v>0.435</v>
       </c>
       <c r="S20">
-        <v>5.3</v>
+        <v>5</v>
       </c>
       <c r="T20">
-        <v>6.9</v>
+        <v>6.4</v>
       </c>
       <c r="U20">
-        <v>0.772</v>
+        <v>0.78</v>
       </c>
       <c r="V20">
         <v>0.8</v>
@@ -5352,22 +5352,22 @@
         <v>7.4</v>
       </c>
       <c r="Z20">
-        <v>1.1</v>
+        <v>1.3</v>
       </c>
       <c r="AA20">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="AB20">
-        <v>2.3</v>
+        <v>2.4</v>
       </c>
       <c r="AC20">
         <v>2.8</v>
       </c>
       <c r="AD20">
-        <v>26.3</v>
+        <v>24.4</v>
       </c>
       <c r="AF20">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AG20">
         <v>122</v>
@@ -5392,13 +5392,13 @@
         <v>49</v>
       </c>
       <c r="G22">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="H22">
         <v>169</v>
       </c>
       <c r="I22">
-        <v>7910</v>
+        <v>7953</v>
       </c>
       <c r="J22">
         <v>7.1</v>
@@ -5407,16 +5407,16 @@
         <v>19</v>
       </c>
       <c r="L22">
-        <v>0.373</v>
+        <v>0.372</v>
       </c>
       <c r="M22">
-        <v>4.6</v>
+        <v>4.5</v>
       </c>
       <c r="N22">
-        <v>12.8</v>
+        <v>12.7</v>
       </c>
       <c r="O22">
-        <v>0.358</v>
+        <v>0.356</v>
       </c>
       <c r="P22">
         <v>2.5</v>
@@ -5425,7 +5425,7 @@
         <v>6.2</v>
       </c>
       <c r="R22">
-        <v>0.405</v>
+        <v>0.404</v>
       </c>
       <c r="S22">
         <v>3.5</v>
@@ -5434,7 +5434,7 @@
         <v>4.3</v>
       </c>
       <c r="U22">
-        <v>0.8149999999999999</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="V22">
         <v>0.8</v>
@@ -5576,16 +5576,16 @@
         <v>-3.6</v>
       </c>
       <c r="L24">
-        <v>-0.03999999999999998</v>
+        <v>-0.03899999999999998</v>
       </c>
       <c r="M24">
-        <v>-0.2999999999999998</v>
+        <v>-0.2000000000000002</v>
       </c>
       <c r="N24">
-        <v>-0.8000000000000007</v>
+        <v>-0.6999999999999993</v>
       </c>
       <c r="O24">
-        <v>-0.001000000000000001</v>
+        <v>0.001000000000000001</v>
       </c>
       <c r="P24">
         <v>-1.6</v>
@@ -5594,7 +5594,7 @@
         <v>-2.8</v>
       </c>
       <c r="R24">
-        <v>-0.155</v>
+        <v>-0.154</v>
       </c>
       <c r="S24">
         <v>2.5</v>
@@ -5603,7 +5603,7 @@
         <v>2.600000000000001</v>
       </c>
       <c r="U24">
-        <v>0.06000000000000005</v>
+        <v>0.05900000000000005</v>
       </c>
       <c r="V24">
         <v>0.8999999999999999</v>
@@ -6289,34 +6289,34 @@
         <v>50</v>
       </c>
       <c r="G11">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H11">
-        <v>1202</v>
+        <v>1245</v>
       </c>
       <c r="I11">
-        <v>13.2</v>
+        <v>12.7</v>
       </c>
       <c r="J11">
-        <v>0.5629999999999999</v>
+        <v>0.554</v>
       </c>
       <c r="K11">
-        <v>0.787</v>
+        <v>0.784</v>
       </c>
       <c r="L11">
-        <v>0.297</v>
+        <v>0.293</v>
       </c>
       <c r="M11">
         <v>1.7</v>
       </c>
       <c r="N11">
-        <v>8.6</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="O11">
         <v>5.1</v>
       </c>
       <c r="P11">
-        <v>19.7</v>
+        <v>19.6</v>
       </c>
       <c r="Q11">
         <v>1.6</v>
@@ -6325,34 +6325,34 @@
         <v>1.1</v>
       </c>
       <c r="S11">
-        <v>9.4</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="T11">
         <v>17.1</v>
       </c>
       <c r="V11">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="W11">
         <v>0.9</v>
       </c>
       <c r="X11">
-        <v>2.6</v>
+        <v>2.5</v>
       </c>
       <c r="Y11">
-        <v>0.102</v>
+        <v>0.095</v>
       </c>
       <c r="AA11">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="AB11">
         <v>-0.1</v>
       </c>
       <c r="AC11">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
       <c r="AD11">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="AE11" t="s">
         <v>51</v>
@@ -6405,7 +6405,7 @@
         <v>5</v>
       </c>
       <c r="P12">
-        <v>18.8</v>
+        <v>18.7</v>
       </c>
       <c r="Q12">
         <v>1.8</v>
@@ -6423,13 +6423,13 @@
         <v>0.9</v>
       </c>
       <c r="W12">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="X12">
         <v>1.7</v>
       </c>
       <c r="Y12">
-        <v>0.101</v>
+        <v>0.103</v>
       </c>
       <c r="AA12">
         <v>-0.4</v>
@@ -6438,7 +6438,7 @@
         <v>0.5</v>
       </c>
       <c r="AC12">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AD12">
         <v>0.4</v>
@@ -6467,70 +6467,70 @@
         <v>50</v>
       </c>
       <c r="G13">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H13">
-        <v>391</v>
+        <v>434</v>
       </c>
       <c r="I13">
-        <v>16</v>
+        <v>14.5</v>
       </c>
       <c r="J13">
-        <v>0.589</v>
+        <v>0.5659999999999999</v>
       </c>
       <c r="K13">
-        <v>0.736</v>
+        <v>0.733</v>
       </c>
       <c r="L13">
-        <v>0.358</v>
+        <v>0.343</v>
       </c>
       <c r="M13">
-        <v>1.9</v>
+        <v>1.7</v>
       </c>
       <c r="N13">
-        <v>9.1</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="O13">
         <v>5.3</v>
       </c>
       <c r="P13">
-        <v>21.7</v>
+        <v>21.4</v>
       </c>
       <c r="Q13">
-        <v>1.1</v>
+        <v>1.3</v>
       </c>
       <c r="R13">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="S13">
-        <v>9.4</v>
+        <v>10</v>
       </c>
       <c r="T13">
-        <v>21.5</v>
+        <v>21</v>
       </c>
       <c r="V13">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="W13">
         <v>0.1</v>
       </c>
       <c r="X13">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="Y13">
-        <v>0.104</v>
+        <v>0.079</v>
       </c>
       <c r="AA13">
-        <v>3.1</v>
+        <v>1.7</v>
       </c>
       <c r="AB13">
-        <v>-1.3</v>
+        <v>-1.4</v>
       </c>
       <c r="AC13">
-        <v>1.8</v>
+        <v>0.2</v>
       </c>
       <c r="AD13">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="AE13" t="s">
         <v>51</v>
@@ -6688,7 +6688,7 @@
         <v>2.5</v>
       </c>
       <c r="W17">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="X17">
         <v>4.5</v>
@@ -6706,7 +6706,7 @@
         <v>-0.7</v>
       </c>
       <c r="AD17">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="AE17" t="s">
         <v>51</v>
@@ -6839,7 +6839,7 @@
         <v>-2.4</v>
       </c>
       <c r="W19">
-        <v>-2</v>
+        <v>-2.1</v>
       </c>
       <c r="X19">
         <v>-4.4</v>
@@ -6857,7 +6857,7 @@
         <v>-0.4000000000000001</v>
       </c>
       <c r="AD19">
-        <v>-0.9</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="20" spans="1:31">
@@ -6874,70 +6874,70 @@
         <v>49</v>
       </c>
       <c r="G20">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H20">
-        <v>391</v>
+        <v>434</v>
       </c>
       <c r="I20">
-        <v>16</v>
+        <v>14.5</v>
       </c>
       <c r="J20">
-        <v>0.589</v>
+        <v>0.5659999999999999</v>
       </c>
       <c r="K20">
-        <v>0.736</v>
+        <v>0.733</v>
       </c>
       <c r="L20">
-        <v>0.358</v>
+        <v>0.343</v>
       </c>
       <c r="M20">
-        <v>1.9</v>
+        <v>1.7</v>
       </c>
       <c r="N20">
-        <v>9.1</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="O20">
         <v>5.3</v>
       </c>
       <c r="P20">
-        <v>21.7</v>
+        <v>21.4</v>
       </c>
       <c r="Q20">
-        <v>1.1</v>
+        <v>1.3</v>
       </c>
       <c r="R20">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="S20">
-        <v>9.4</v>
+        <v>10</v>
       </c>
       <c r="T20">
-        <v>21.5</v>
+        <v>21</v>
       </c>
       <c r="V20">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="W20">
         <v>0.1</v>
       </c>
       <c r="X20">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="Y20">
-        <v>0.104</v>
+        <v>0.079</v>
       </c>
       <c r="AA20">
-        <v>3.1</v>
+        <v>1.7</v>
       </c>
       <c r="AB20">
-        <v>-1.3</v>
+        <v>-1.4</v>
       </c>
       <c r="AC20">
-        <v>1.8</v>
+        <v>0.2</v>
       </c>
       <c r="AD20">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="AE20" t="s">
         <v>51</v>
@@ -6959,19 +6959,19 @@
         <v>49</v>
       </c>
       <c r="G22">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="H22">
-        <v>7910</v>
+        <v>7953</v>
       </c>
       <c r="I22">
-        <v>13.7</v>
+        <v>13.6</v>
       </c>
       <c r="J22">
-        <v>0.533</v>
+        <v>0.531</v>
       </c>
       <c r="K22">
-        <v>0.672</v>
+        <v>0.673</v>
       </c>
       <c r="L22">
         <v>0.227</v>
@@ -6980,7 +6980,7 @@
         <v>1.8</v>
       </c>
       <c r="N22">
-        <v>8.199999999999999</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="O22">
         <v>4.9</v>
@@ -6995,22 +6995,22 @@
         <v>0.6</v>
       </c>
       <c r="S22">
-        <v>11.7</v>
+        <v>11.8</v>
       </c>
       <c r="T22">
         <v>20.8</v>
       </c>
       <c r="V22">
-        <v>8.300000000000001</v>
+        <v>8.1</v>
       </c>
       <c r="W22">
-        <v>4.3</v>
+        <v>4.4</v>
       </c>
       <c r="X22">
-        <v>12.6</v>
+        <v>12.5</v>
       </c>
       <c r="Y22">
-        <v>0.077</v>
+        <v>0.076</v>
       </c>
       <c r="AA22">
         <v>1</v>
@@ -7022,7 +7022,7 @@
         <v>-0.3</v>
       </c>
       <c r="AD22">
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
       <c r="AE22" t="s">
         <v>51</v>
@@ -7113,13 +7113,13 @@
         <v>22</v>
       </c>
       <c r="I24">
-        <v>-2.199999999999999</v>
+        <v>-2.1</v>
       </c>
       <c r="J24">
-        <v>0.02500000000000002</v>
+        <v>0.02700000000000002</v>
       </c>
       <c r="K24">
-        <v>0.106</v>
+        <v>0.105</v>
       </c>
       <c r="L24">
         <v>0.217</v>
@@ -7128,7 +7128,7 @@
         <v>1.9</v>
       </c>
       <c r="N24">
-        <v>6.5</v>
+        <v>6.399999999999999</v>
       </c>
       <c r="O24">
         <v>4</v>
@@ -7143,22 +7143,22 @@
         <v>0.7999999999999999</v>
       </c>
       <c r="S24">
-        <v>4</v>
+        <v>3.899999999999999</v>
       </c>
       <c r="T24">
         <v>-2.5</v>
       </c>
       <c r="V24">
-        <v>-8.200000000000001</v>
+        <v>-8</v>
       </c>
       <c r="W24">
-        <v>-4.3</v>
+        <v>-4.4</v>
       </c>
       <c r="X24">
-        <v>-12.5</v>
+        <v>-12.4</v>
       </c>
       <c r="Y24">
-        <v>-0.028</v>
+        <v>-0.027</v>
       </c>
       <c r="AA24">
         <v>-1.2</v>
@@ -7170,7 +7170,7 @@
         <v>-0.8</v>
       </c>
       <c r="AD24">
-        <v>-3.4</v>
+        <v>-3.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>